<commit_message>
update WA state datafile
</commit_message>
<xml_diff>
--- a/Data/Raw/fe_newnames.xlsx
+++ b/Data/Raw/fe_newnames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\fewapo\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7FBA09-7E97-4AB4-B51D-573E81CD1299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F6BED1-B5A3-49DE-8688-3FB1A564EB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fe-newnames.xlsx" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="824">
   <si>
     <t>Unique ID</t>
   </si>
@@ -2009,6 +2009,493 @@
   </si>
   <si>
     <t>https://www.kptv.com/2024/03/01/clark-co-sheriff-releases-video-moment-deputies-shot-killed-suspect-brush-prairie/</t>
+  </si>
+  <si>
+    <t>https://komonews.com/news/local/woman-killed-sr525-wrong-way-crash-lynnwood-snohomish-county-deputies-domestic-violence-kidnapping-suspect-pursuit</t>
+  </si>
+  <si>
+    <t>Trudy Slanger</t>
+  </si>
+  <si>
+    <t>14800 State Route 525</t>
+  </si>
+  <si>
+    <t>Snohomish County Sheriff's Office</t>
+  </si>
+  <si>
+    <t>Sheriff's deputies were pursuing a  man in connection to a domestic violence assault and kidnapping of a woman who was in his truck.  They terminated as he started driving the wrong way on State Route 525 just before the crash.  His truck hit a SUV head-on, killing the driver and seriously injuring himself and the passenger in his car.</t>
+  </si>
+  <si>
+    <t>14000 NE 20th Ave</t>
+  </si>
+  <si>
+    <t>Deputies responded to two reported carjackings, and tracked the suspect to an American Legion building, where they shot him.  A witness said that the he realized the suspect was armed when he raised his arms.</t>
+  </si>
+  <si>
+    <t>Alan Jenks</t>
+  </si>
+  <si>
+    <t>1800 West Dean</t>
+  </si>
+  <si>
+    <t>https://www.krem.com/article/news/crime/spokane-arson-police-shooting-victim-identity/293-ff0bcc77-d49d-40fb-9dd4-64592221ca27</t>
+  </si>
+  <si>
+    <t>Spokane police officers were responding to a suspicious house fire. Police claim Jenks was not cooperative while being interviewed about the incident and tried to walk away during questioning.  Officers tried to detain Jenks, at which point police say he shot a gun he was carrying and two officers shot back and killed him on the scene.  Another man was arrested and charged with arson for starting the fire.</t>
+  </si>
+  <si>
+    <t>Lynnwood</t>
+  </si>
+  <si>
+    <t>Benjamin Steven Woods</t>
+  </si>
+  <si>
+    <t>https://www.columbian.com/news/2024/apr/17/prineville-man-shot-multiple-times-by-clark-county-sheriffs-deputies-in-salmon-creek-says-medical-examiner/</t>
+  </si>
+  <si>
+    <t>https://www.king5.com/article/news/crime/man-killed-by-police-tukwila-hotel-believed-he-was-meeting-girls-under-12/281-03098558-b006-4a14-866c-7ceb3f7fc374</t>
+  </si>
+  <si>
+    <t>16500 Southcenter Pkwy</t>
+  </si>
+  <si>
+    <t>Officers were conducting an operation at the hotel as part of the department's Internet Crimes Against Children Taskforce.  Bodycam video shows them opening the door to confront the suspect, when he pulls a handgun out of his jacket they shoot and kill him.</t>
+  </si>
+  <si>
+    <t>Bruce Coval Meneley</t>
+  </si>
+  <si>
+    <t>Officers Adam Fowler, Officer Nicholas French</t>
+  </si>
+  <si>
+    <t>https://www.thestranger.com/slog-am/2024/04/24/79483588/slog-am-first-seattle-police-shooting-this-year-supreme-court-hears-idaho-abortion-case-senate-passes-tiktok-ban?utm_source=Stranger%2FMercury%2FEverOut&amp;utm_campaign=b0c08e7248-EMAIL_CAMPAIGN_2023_02_09_08_31_COPY_01&amp;utm_medium=email&amp;utm_term=0_-a7406d5101-%5BLIST_EMAIL_ID%5D</t>
+  </si>
+  <si>
+    <t>Tukwila</t>
+  </si>
+  <si>
+    <t>Sgt Fred Harrison, Deputy Enrique Cordero; Deputy Jim Payne; Deputy Michael Gonzalez</t>
+  </si>
+  <si>
+    <t>Spokane County Sherrif's Office</t>
+  </si>
+  <si>
+    <t>30300 North Monroe Road</t>
+  </si>
+  <si>
+    <t>Spokane County Sheriff’s Office specialty units responded to assist the Stevens County Sheriff’s Office with arresting Hegel, who had failed to show up to court earlier in the week.  After attempting to deescalate the situation, deputies deployed chemical munitions into the residence to force him to come out, but he did not.  They eventually forced open the home’s front door and allegedly responded to an immediate threat by shooting and killing him.</t>
+  </si>
+  <si>
+    <t>https://www.spokesman.com/stories/2024/apr/03/man-shot-by-deputies-near-deer-park-had-standoff-w/</t>
+  </si>
+  <si>
+    <t>Deputy Josiah Loos, Detectives Samuel Turner and Travis West</t>
+  </si>
+  <si>
+    <t>https://www.khq.com/news/3-spokane-county-deputies-who-shot-and-killed-a-child-rape-suspect-named/article_a0019890-f383-11ee-aae2-a70786480827.html</t>
+  </si>
+  <si>
+    <t>Donald Hegel</t>
+  </si>
+  <si>
+    <t>Joseph Jacob Hadden</t>
+  </si>
+  <si>
+    <t>101 W. Front St</t>
+  </si>
+  <si>
+    <t>Port Angeles</t>
+  </si>
+  <si>
+    <t>Port Angeles Police Department</t>
+  </si>
+  <si>
+    <t>Two Port Angeles police officers responded to a bank hold-up alarm May 3 and encountered ths subject, who allegedly had a handgun.  They shot and killed him.</t>
+  </si>
+  <si>
+    <t>https://www.msn.com/en-us/news/crime/investigators-seeking-woman-who-used-atm/ar-BB1mWN0b</t>
+  </si>
+  <si>
+    <t>Marvin Arellano</t>
+  </si>
+  <si>
+    <t>I5 exit 195</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>WSP troopers shot and killed a man who was likely having a manic episode and had attacked two construction workers after getting stuck behind their vehicle on I5.</t>
+  </si>
+  <si>
+    <t>https://apnews.com/article/police-shoot-idaho-man-washington-freeway-a781bf295af8c5c4faca692d6e615f7b</t>
+  </si>
+  <si>
+    <t>Salih Beslic</t>
+  </si>
+  <si>
+    <t>Machete</t>
+  </si>
+  <si>
+    <t>https://www.tri-cityherald.com/news/local/crime/article288917692.html</t>
+  </si>
+  <si>
+    <t>Detective TJ Orth</t>
+  </si>
+  <si>
+    <t>3300 W Court St</t>
+  </si>
+  <si>
+    <t>Police were called to respond to a man allegedly wielding a machete.  When he allegedly charged at the officers he was shot and killed.</t>
+  </si>
+  <si>
+    <t>Michael Aaron Vaughn</t>
+  </si>
+  <si>
+    <t>https://www.kentreporter.com/northwest/man-killed-by-sheriffs-deputies-in-auburn-identified/</t>
+  </si>
+  <si>
+    <t>24 Auburn Way South</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>King County Sheriff's Office, Auburn Police Department</t>
+  </si>
+  <si>
+    <t>Vaughn was shot and killed by police during an eviction.</t>
+  </si>
+  <si>
+    <t>https://www.columbian.com/news/2024/jun/25/four-vancouver-police-officers-identified-in-early-morning-fatal-shooting-on-andresen-road/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seargant  James Kelly, Officers Jason Haigwood, Justin Reiner and Philip Wilkening </t>
+  </si>
+  <si>
+    <t>Jonathan West Nelson</t>
+  </si>
+  <si>
+    <t>2400 Northeast Andresen Road</t>
+  </si>
+  <si>
+    <t>https://www.columbian.com/news/2024/jun/20/40-year-old-vancouver-man-fatally-shot-by-police-on-andresen-road-identified/</t>
+  </si>
+  <si>
+    <t>Police were responding to a report of a man with a gun.  They shot him after he allegedly pointed the firearm at him.</t>
+  </si>
+  <si>
+    <t>https://www.cityofvancouver.us/vancouver-police-involved-in-shooting/</t>
+  </si>
+  <si>
+    <t>https://www.cityofvancouver.us/vancouver-police-officer-involved-in-shooting/</t>
+  </si>
+  <si>
+    <t>Police were responding to a report of a man with and aggressive dog and a gun.  They shot him after he allegedly pointed the firearm at him.</t>
+  </si>
+  <si>
+    <t>https://www.clarkcountytoday.com/news/vancouver-police-officers-identified-in-june-8-shooting/</t>
+  </si>
+  <si>
+    <t>Officer Brandon Riedel</t>
+  </si>
+  <si>
+    <t>Vadim V. Sashchenko</t>
+  </si>
+  <si>
+    <t>100 block of SE Columbia Way</t>
+  </si>
+  <si>
+    <t>Deer Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 205th St E and 6th Ave Ct E.</t>
+  </si>
+  <si>
+    <t>Police were pursuing a subject who did not respond to an attempted traffic stop.  The subject allegedly shot at police both during the chase, and after he was cornered in his neighborhood.  They returned fire, killing him.</t>
+  </si>
+  <si>
+    <t>https://komonews.com/news/local/pierce-county-spanaway-officer-involved-shooting-ois-sheriffs-office-deputies-police-officers-washington-state-patrol-troopers-shooting-gunshot-shot-freeway-i5-tacoma-suspect-condition-law-enforcement</t>
+  </si>
+  <si>
+    <t>https://www.seattletimes.com/seattle-news/law-justice/pierce-county-deputies-fatally-shoot-person-near-spanaway/</t>
+  </si>
+  <si>
+    <t>Police were pursuing a stolen car.   The driver crashed while fleeing.  The passenger in his car, a 14-year-old girl, was injured and the driver of the other car was severely injured and died a few days later.</t>
+  </si>
+  <si>
+    <t>4400 Airport Way South</t>
+  </si>
+  <si>
+    <t>https://www.kiro7.com/news/one-dead-after-high-speed-car-chase-next-boeing-airfield/7NE75LCJKNCI5JEDMIYNO54P7M/</t>
+  </si>
+  <si>
+    <t>Ivan Zaytsev</t>
+  </si>
+  <si>
+    <t>Jonathan Luksan</t>
+  </si>
+  <si>
+    <t>Dante Cudini</t>
+  </si>
+  <si>
+    <t>Christian Demetri Moshofsky</t>
+  </si>
+  <si>
+    <t>102 Madison Ave</t>
+  </si>
+  <si>
+    <t>242nd Avenue Court East</t>
+  </si>
+  <si>
+    <t>4800 33rd Avenue Court East</t>
+  </si>
+  <si>
+    <t>Colville</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Stevens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+260th St. E and 70th Ave</t>
+  </si>
+  <si>
+    <t>Stevens County Sheriff's Office</t>
+  </si>
+  <si>
+    <t>Highway 395 and Auto View Road</t>
+  </si>
+  <si>
+    <t>Lois K Phair</t>
+  </si>
+  <si>
+    <t>KCME deaths 8/9/2024</t>
+  </si>
+  <si>
+    <t>https://www.statesmanexaminer.com/news/local/suspect-in-attack-on-prosecutor-named/article_0aec85f2-54d7-11ef-9761-43a632b11302.html</t>
+  </si>
+  <si>
+    <t>The subject had allegedly attacked a deputy prosecutor after a court hearing and fled.  He was located and stopped by a sheriff's deputy, and allegedly exited his van and charged the deputy with a machete in his hand. The deputy shot and killed him.</t>
+  </si>
+  <si>
+    <t>Sheriff's deputies were responding to a domestic incident involving a weapon.  The man allegedly pointed his weapon at the deputies, and three of them shot and killed him.</t>
+  </si>
+  <si>
+    <t>https://www.piercecountywa.gov/DocumentCenter/View/139933/PCFIT-PCSD-August-23-2024</t>
+  </si>
+  <si>
+    <t>https://mynorthwest.com/3969687/man-killed-in-pierce-county-deputy-involved-shooting/</t>
+  </si>
+  <si>
+    <t>https://www.chronline.com/stories/38-year-old-man-killed-by-pierce-county-deputies-during-pursuit-officially-identified,347721</t>
+  </si>
+  <si>
+    <t>The subject was was shot and killed by Pierce County deputies following a pursuit.  The reason for the initial pursuit was not released, but the subject was described as a "criminal suspect".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26100 104th Avenue Southeast</t>
+  </si>
+  <si>
+    <t>Alizar A. Kachiyev</t>
+  </si>
+  <si>
+    <t>https://ilovekent.net/teen-driver-charged-as-adult-in-july-13-fatal-kent-crash/</t>
+  </si>
+  <si>
+    <t>Deputies responded to a domestic-violence call involving an argument among family members. The 911 caller said their brother had a knife. Deputies contacted the man, he ran to a shed on the property and they reported, “Shots fired,” over the radio shortly after.</t>
+  </si>
+  <si>
+    <t>Kent police said officers were responding to a 911 call of shots fired when they heard more gunshots they believed had been fired at them from the upper story of a nearby building, and one officer fired a gun in that direction.  Officers then detained someone who said their brother, believed to be subject, had shot himself. However, a Port of Seattle Police Department spokesperson said investigators “don’t have conclusive answers” as to whether the subject was killed by a police officer.  The King County prosecutors office listed this as a use of force fatality.</t>
+  </si>
+  <si>
+    <t>https://www.seattletimes.com/seattle-news/law-justice/details-on-mans-death-still-unclear-after-he-exchanged-gunfire-with-kent-police/</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>https://www.kentreporter.com/news/mother-of-man-fatally-shot-in-kent-starts-fundraiser-for-funeral/</t>
+  </si>
+  <si>
+    <t>https://www.dignitymemorial.com/obituaries/seattle-wa/lois-phair-11943544</t>
+  </si>
+  <si>
+    <t>WSP were pursuing a driver who fled from multiple attempts to stop her for expired registration tags.  The driver allegedly rammed the trooper's vehicle, sped off and crashed into a power pole, killing the passenger.  Troopers claim they were not actively pursuing the vehicle when it hit the light pole.</t>
+  </si>
+  <si>
+    <t>Gina Munna</t>
+  </si>
+  <si>
+    <t>https://www.wsaz.com/2024/09/10/grandmother-70-dies-head-on-crash-with-driver-allegedly-trying-flee-deputies/</t>
+  </si>
+  <si>
+    <t>The subject was being pursued by deputies for a suspected stolen car and drug-related behavior, through Lacey and Olympia.  Eventually she collided with another car, killing one of the occupants and injuring two others.</t>
+  </si>
+  <si>
+    <t>Fones Rd and Pacific Avenue</t>
+  </si>
+  <si>
+    <t>Snohomish Couty Sheriff's Office</t>
+  </si>
+  <si>
+    <t>https://www.seattletimes.com/seattle-news/suspect-killed-after-snohomish-county-deputies-chase-ram-vehicle/</t>
+  </si>
+  <si>
+    <t>7500 Hiway 9</t>
+  </si>
+  <si>
+    <t>The subject was being pursued by deputies for a suspected homicide.  They tried stopping the suspect with a PIT maneuver, using their patrol car to push the rear-end of a fleeing vehicle sideways and causing it to spin out. The man was thrown from the vehicle and died at the scene.</t>
+  </si>
+  <si>
+    <t>Sumner</t>
+  </si>
+  <si>
+    <t>Sumner Police Department, Puyallup Police Department, Bonney Lake Police Department</t>
+  </si>
+  <si>
+    <t>Sumner police were dispatched to investigate a man in crisis on the railroad tracks. The man was allegedly armed with a knife. Washington State Patrol, the Puyallup Police Department, Bonney Lake Police Department and a civilian crisis responder provided assistance. The man was shot and killed by officers from 3 different departments after about 2 hours.  The man who originally called 911 said he would never have called if he had known what would happen.</t>
+  </si>
+  <si>
+    <t>https://www.fox13seattle.com/news/person-fatally-shot-police-sumner</t>
+  </si>
+  <si>
+    <t>900 Traffic Avenue</t>
+  </si>
+  <si>
+    <t>Kody Dean Olsen</t>
+  </si>
+  <si>
+    <t>https://komonews.com/news/local/maple-valley-bodies-found-arrest-charges-seattle-tacoma-washington-king-pierce-county-brandon-gerner-joshua-jones-kody-olsen-suspects-jail-victims-robert-riley-ashley-williams-shootout-deputies-officer-involved-shooting-crime-crisis-animal-horse-lemon</t>
+  </si>
+  <si>
+    <t>4300 Vickery Ave E</t>
+  </si>
+  <si>
+    <t>Deputies attempted a traffic stop for a suspected DUI but the subject fled.  At some point he allegedly shot at the deputies and they fired back.  He was eventually pulled from the vehicle and transported to hospital where he died several days later.</t>
+  </si>
+  <si>
+    <t>https://komonews.com/news/local/tacoma-standoff-shooting-dui-suspect-bullet-hits-pierce-county-deputy-handcuff-belt-uninjured-4300-vickery-ave-east-ois</t>
+  </si>
+  <si>
+    <t>https://www.piercecountywa.gov/DocumentCenter/View/134569/January-12-2024-PCFIT-4300-Vickery-Avenue</t>
+  </si>
+  <si>
+    <t>Timothy McDonald</t>
+  </si>
+  <si>
+    <t>Jeffery Kiner</t>
+  </si>
+  <si>
+    <t>https://www.thenewstribune.com/news/local/crime/article289697439.html</t>
+  </si>
+  <si>
+    <t>https://www.piercecountywa.gov/DocumentCenter/View/138570/July-5-2024-PCFIT-4800-33rd-Ave-Ct-E</t>
+  </si>
+  <si>
+    <t>Charles Ferree</t>
+  </si>
+  <si>
+    <t>Deolia Blandford</t>
+  </si>
+  <si>
+    <t>Highway 101 and SE Lynch Road</t>
+  </si>
+  <si>
+    <t>Shelton</t>
+  </si>
+  <si>
+    <t>Mason</t>
+  </si>
+  <si>
+    <t>The victim was attempting to make a turn when the trooper who was traveling at a high rate of speed to a vehicle fire at an exit of the highway 101, reportedly with lights and siren activated, collided with the victim's vehicle, killing both the victim and his passenger.</t>
+  </si>
+  <si>
+    <t>The victim was a passenger in a vehicle attempting to make a turn when the trooper who was traveling at a high rate of speed to a vehicle fire at an exit of the highway 101, reportedly with lights and siren activated, collided with the vehicle, killing both the victim and the driver.</t>
+  </si>
+  <si>
+    <t>Vehicle Accident</t>
+  </si>
+  <si>
+    <t>https://www.thenewstribune.com/news/local/article287454220.html</t>
+  </si>
+  <si>
+    <t>Gabriel Daniel Renteria</t>
+  </si>
+  <si>
+    <t>Native American</t>
+  </si>
+  <si>
+    <t>I5 milepost 190</t>
+  </si>
+  <si>
+    <t>Police responded to a report of shots fired and found one person dead and another critically injured.  Based on local witness descriptions they located the alleged suspect and pursued him onto I5, where he crashed, involving other vehicles.  Police allege he then shot himself.</t>
+  </si>
+  <si>
+    <t>John Robinson</t>
+  </si>
+  <si>
+    <t>Yelm Police Department, Nisqually Tribal Police Department, Thurston County Sheriff's Office</t>
+  </si>
+  <si>
+    <t>4600 Herman Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Police pursued the subject who fled for some distance before losing control over his motorcyle on a gravel driveway, crashed and was killed. </t>
+  </si>
+  <si>
+    <t>ME_url</t>
+  </si>
+  <si>
+    <t>https://www.piercecountywa.gov/CivicAlerts.aspx?AID=6540</t>
+  </si>
+  <si>
+    <t>Vancouver Police Department, Clark County Sheriff's Office, SWAT</t>
+  </si>
+  <si>
+    <t>Police responded to reports of a man threatening his neighbors.  They arrived with a drone and an armored vehicle.  The man allegedly had a gun and a rifle and shot at the armed vehicle.  After a 3 hour standoff, he was shot and killed</t>
+  </si>
+  <si>
+    <t>https://www.seattletimes.com/seattle-news/law-justice/wsp-pursuit-ends-in-deadly-crash-in-everett/</t>
+  </si>
+  <si>
+    <t>"Another neighbor, Selene Gudino, said she is grateful her family was not hurt. She explained she had parked in her driveway with her kids in the car within seconds of the crash just a few hundred feet away." https://www.msn.com/en-us/news/crime/state-patrol-pursuit-leads-to-deadly-rollover-crash-in-everett/ar-AA1rrstK Komo News</t>
+  </si>
+  <si>
+    <t>1900 Rainier Avenue</t>
+  </si>
+  <si>
+    <t>name not released due to suicide</t>
+  </si>
+  <si>
+    <t>https://snohomishcountywa.gov/ArchiveCenter/ViewFile/Item/7216</t>
+  </si>
+  <si>
+    <t>https://www.theolympian.com/news/local/article292881774.html</t>
+  </si>
+  <si>
+    <t>https://www.heraldnet.com/news/police-chase-ends-in-fatal-crash-in-everett/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington State Patrol initiated the pursuit along Highway 2 near Lake Stevens, which then continued into Everett.  What led to the pursuit is still not known.  The chase ended in a residential neighborhood with a fatal rollover crash.  </t>
+  </si>
+  <si>
+    <t>Elicio Paco Sanorico-Bocanegra</t>
+  </si>
+  <si>
+    <t>https://www.heraldnet.com/news/everett-double-shooting-victim-and-suspect-both-18-identified/</t>
+  </si>
+  <si>
+    <t>https://www.oregonlive.com/crime/2024/10/man-shot-to-death-by-vancouver-police-during-standoff-in-september-identified.html</t>
+  </si>
+  <si>
+    <t>Michael D. Williams</t>
+  </si>
+  <si>
+    <t>5400 NE 71st st</t>
   </si>
 </sst>
 </file>
@@ -2322,7 +2809,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2437,6 +2924,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2483,7 +2981,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2491,8 +2989,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2539,7 +3036,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="33">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2651,39 +3151,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AD103" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:AD103" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Unique ID" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Age" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Gender" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Race" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date of injury resulting in death (month/day/year)" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Location of injury (address)" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Location of death (city)" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="State" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Location of death (zip code)" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Location of death (county)" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Latitude" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Longitude" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Agency or agencies involved" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Highest level of force" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Armed/Unarmed" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Alleged weapon" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Fleeing/Not fleeing" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Brief description" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Dispositions/Exclusions INTERNAL USE, NOT FOR ANALYSIS" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Intended use of force (Developing)" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Supporting document link" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Foreknowledge of mental illness? INTERNAL USE, NOT FOR ANALYSIS" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="MH Crisis" dataDxfId="6"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Notes" dataDxfId="5"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="additional_url" dataDxfId="4"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="officer_names" dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="officer_url" dataDxfId="2"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="victim_url" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IIT_url" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AE132" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:AE132" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD128">
+    <sortCondition ref="A1:A128"/>
+  </sortState>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Unique ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Age" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Gender" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Race" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date of injury resulting in death (month/day/year)" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Location of injury (address)" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Location of death (city)" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="State" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Location of death (zip code)" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Location of death (county)" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Latitude" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Longitude" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Agency or agencies involved" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Highest level of force" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Armed/Unarmed" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Alleged weapon" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Fleeing/Not fleeing" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Brief description" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Dispositions/Exclusions INTERNAL USE, NOT FOR ANALYSIS" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Intended use of force (Developing)" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Supporting document link" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Foreknowledge of mental illness? INTERNAL USE, NOT FOR ANALYSIS" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="MH Crisis" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="additional_url" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="officer_names" dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="officer_url" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="victim_url" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IIT_url" dataDxfId="1"/>
+    <tableColumn id="31" xr3:uid="{D2192FFE-CAEF-48FA-BD54-4E5A331A662B}" name="ME_url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2986,46 +3490,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD103"/>
+  <dimension ref="A1:AE132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB103" sqref="AB103"/>
+      <selection pane="bottomRight" activeCell="A124" sqref="A124:XFD124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" customWidth="1"/>
-    <col min="6" max="6" width="47.54296875" customWidth="1"/>
-    <col min="7" max="7" width="27.1796875" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" customWidth="1"/>
-    <col min="10" max="10" width="27.54296875" customWidth="1"/>
-    <col min="11" max="11" width="26.26953125" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="18.1796875" customWidth="1"/>
-    <col min="17" max="17" width="17.54296875" customWidth="1"/>
-    <col min="18" max="18" width="20.54296875" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" customWidth="1"/>
-    <col min="20" max="20" width="54.54296875" customWidth="1"/>
-    <col min="21" max="21" width="34.1796875" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1"/>
+    <col min="18" max="18" width="20.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="20" width="54.5703125" customWidth="1"/>
+    <col min="21" max="21" width="34.140625" customWidth="1"/>
     <col min="22" max="22" width="26" customWidth="1"/>
-    <col min="23" max="23" width="63.7265625" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" customWidth="1"/>
-    <col min="26" max="26" width="15.54296875" customWidth="1"/>
-    <col min="27" max="27" width="15.81640625" customWidth="1"/>
-    <col min="28" max="28" width="12.453125" customWidth="1"/>
+    <col min="23" max="23" width="63.7109375" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="15.5703125" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" customWidth="1"/>
     <col min="29" max="29" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3116,8 +3620,11 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AE1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>90001</v>
       </c>
@@ -3176,7 +3683,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>90002</v>
       </c>
@@ -3244,7 +3751,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>90003</v>
       </c>
@@ -3306,7 +3813,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>90004</v>
       </c>
@@ -3368,7 +3875,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90005</v>
       </c>
@@ -3439,7 +3946,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>90006</v>
       </c>
@@ -3498,7 +4005,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>90007</v>
       </c>
@@ -3569,7 +4076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>90008</v>
       </c>
@@ -3637,7 +4144,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90009</v>
       </c>
@@ -3702,7 +4209,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90010</v>
       </c>
@@ -3770,7 +4277,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>90011</v>
       </c>
@@ -3841,7 +4348,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>90012</v>
       </c>
@@ -3912,7 +4419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>90013</v>
       </c>
@@ -3971,7 +4478,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>90014</v>
       </c>
@@ -4033,7 +4540,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>90015</v>
       </c>
@@ -4095,7 +4602,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>90016</v>
       </c>
@@ -4160,7 +4667,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>90017</v>
       </c>
@@ -4219,7 +4726,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>90018</v>
       </c>
@@ -4284,7 +4791,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90019</v>
       </c>
@@ -4343,7 +4850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90020</v>
       </c>
@@ -4411,7 +4918,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>90021</v>
       </c>
@@ -4482,7 +4989,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>90022</v>
       </c>
@@ -4547,7 +5054,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>90023</v>
       </c>
@@ -4621,7 +5128,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>90024</v>
       </c>
@@ -4692,7 +5199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90025</v>
       </c>
@@ -4754,7 +5261,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>90026</v>
       </c>
@@ -4822,7 +5329,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>90027</v>
       </c>
@@ -4881,7 +5388,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>90028</v>
       </c>
@@ -4952,7 +5459,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>90029</v>
       </c>
@@ -5020,7 +5527,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>90030</v>
       </c>
@@ -5097,7 +5604,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>90031</v>
       </c>
@@ -5156,7 +5663,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>90032</v>
       </c>
@@ -5230,7 +5737,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>90033</v>
       </c>
@@ -5295,7 +5802,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>90034</v>
       </c>
@@ -5369,7 +5876,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>90035</v>
       </c>
@@ -5434,7 +5941,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>90036</v>
       </c>
@@ -5493,7 +6000,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>90037</v>
       </c>
@@ -5549,7 +6056,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>90038</v>
       </c>
@@ -5617,7 +6124,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>90039</v>
       </c>
@@ -5685,7 +6192,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>90040</v>
       </c>
@@ -5750,7 +6257,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>90041</v>
       </c>
@@ -5809,7 +6316,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>90042</v>
       </c>
@@ -5868,7 +6375,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>90043</v>
       </c>
@@ -5927,7 +6434,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90044</v>
       </c>
@@ -5992,7 +6499,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90045</v>
       </c>
@@ -6054,7 +6561,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>90046</v>
       </c>
@@ -6122,7 +6629,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>90047</v>
       </c>
@@ -6187,7 +6694,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>90048</v>
       </c>
@@ -6249,7 +6756,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>90049</v>
       </c>
@@ -6314,7 +6821,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>90050</v>
       </c>
@@ -6376,7 +6883,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>90051</v>
       </c>
@@ -6438,7 +6945,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>90052</v>
       </c>
@@ -6497,7 +7004,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>90053</v>
       </c>
@@ -6553,7 +7060,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>90054</v>
       </c>
@@ -6612,7 +7119,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>90055</v>
       </c>
@@ -6677,7 +7184,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>90056</v>
       </c>
@@ -6733,7 +7240,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>90057</v>
       </c>
@@ -6792,7 +7299,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>90058</v>
       </c>
@@ -6857,7 +7364,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>90059</v>
       </c>
@@ -6919,7 +7426,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>90060</v>
       </c>
@@ -6978,7 +7485,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>90061</v>
       </c>
@@ -7034,7 +7541,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>90062</v>
       </c>
@@ -7096,7 +7603,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>90063</v>
       </c>
@@ -7158,7 +7665,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>90064</v>
       </c>
@@ -7217,7 +7724,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>90065</v>
       </c>
@@ -7279,7 +7786,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>90066</v>
       </c>
@@ -7341,7 +7848,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>90067</v>
       </c>
@@ -7403,7 +7910,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>90068</v>
       </c>
@@ -7468,7 +7975,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>90069</v>
       </c>
@@ -7533,7 +8040,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>90070</v>
       </c>
@@ -7592,7 +8099,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>90071</v>
       </c>
@@ -7651,7 +8158,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>90072</v>
       </c>
@@ -7713,7 +8220,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>90073</v>
       </c>
@@ -7772,7 +8279,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>90074</v>
       </c>
@@ -7840,7 +8347,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>90075</v>
       </c>
@@ -7902,7 +8409,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>90076</v>
       </c>
@@ -7961,7 +8468,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>90077</v>
       </c>
@@ -8023,7 +8530,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>90078</v>
       </c>
@@ -8079,7 +8586,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>90079</v>
       </c>
@@ -8144,7 +8651,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>90080</v>
       </c>
@@ -8206,7 +8713,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>90081</v>
       </c>
@@ -8268,7 +8775,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>90082</v>
       </c>
@@ -8327,7 +8834,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>90083</v>
       </c>
@@ -8392,7 +8899,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>90084</v>
       </c>
@@ -8454,7 +8961,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>90085</v>
       </c>
@@ -8513,7 +9020,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>90086</v>
       </c>
@@ -8575,7 +9082,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>90087</v>
       </c>
@@ -8637,7 +9144,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>90088</v>
       </c>
@@ -8690,7 +9197,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90089</v>
       </c>
@@ -8764,7 +9271,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90091</v>
       </c>
@@ -8826,7 +9333,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90092</v>
       </c>
@@ -8891,7 +9398,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90093</v>
       </c>
@@ -8953,7 +9460,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>90094</v>
       </c>
@@ -9015,7 +9522,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>90095</v>
       </c>
@@ -9077,7 +9584,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>90096</v>
       </c>
@@ -9139,7 +9646,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>90097</v>
       </c>
@@ -9152,6 +9659,9 @@
       <c r="D97" t="s">
         <v>30</v>
       </c>
+      <c r="E97" t="s">
+        <v>84</v>
+      </c>
       <c r="F97" s="1">
         <v>45322</v>
       </c>
@@ -9207,7 +9717,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>90098</v>
       </c>
@@ -9266,7 +9776,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>90099</v>
       </c>
@@ -9319,7 +9829,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>90100</v>
       </c>
@@ -9384,7 +9894,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>90101</v>
       </c>
@@ -9443,7 +9953,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>90102</v>
       </c>
@@ -9508,77 +10018,1838 @@
         <v>661</v>
       </c>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>90103</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" t="s">
         <v>656</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C103">
         <v>40</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" t="s">
         <v>30</v>
       </c>
       <c r="E103" t="s">
         <v>69</v>
       </c>
-      <c r="F103" s="6">
+      <c r="F103" s="1">
         <v>45369</v>
       </c>
-      <c r="G103" s="5" t="s">
+      <c r="G103" t="s">
         <v>655</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" t="s">
         <v>121</v>
       </c>
-      <c r="I103" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J103" s="5">
+      <c r="I103" t="s">
+        <v>33</v>
+      </c>
+      <c r="J103">
         <v>98404</v>
       </c>
-      <c r="K103" s="5" t="s">
+      <c r="K103" t="s">
         <v>34</v>
       </c>
-      <c r="L103" s="5">
+      <c r="L103">
         <v>47.191309199999999</v>
       </c>
-      <c r="M103" s="5">
+      <c r="M103">
         <v>-122.4191421</v>
       </c>
-      <c r="N103" s="5" t="s">
+      <c r="N103" t="s">
         <v>35</v>
       </c>
-      <c r="O103" s="5" t="s">
+      <c r="O103" t="s">
         <v>36</v>
       </c>
-      <c r="P103" s="5" t="s">
+      <c r="P103" t="s">
         <v>37</v>
       </c>
-      <c r="Q103" s="5" t="s">
+      <c r="Q103" t="s">
         <v>207</v>
       </c>
-      <c r="R103" s="5"/>
-      <c r="S103" s="5" t="s">
+      <c r="S103" t="s">
         <v>657</v>
       </c>
-      <c r="T103" s="5"/>
-      <c r="U103" s="5" t="s">
+      <c r="U103" t="s">
         <v>52</v>
       </c>
       <c r="V103" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="W103" s="5"/>
-      <c r="X103" s="5"/>
-      <c r="Y103" s="5"/>
-      <c r="Z103" s="5"/>
-      <c r="AA103" s="5"/>
-      <c r="AB103" s="5"/>
-      <c r="AC103" s="5"/>
-      <c r="AD103" s="5"/>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>90104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>663</v>
+      </c>
+      <c r="C104">
+        <v>83</v>
+      </c>
+      <c r="D104" t="s">
+        <v>168</v>
+      </c>
+      <c r="F104" s="1">
+        <v>45393</v>
+      </c>
+      <c r="G104" t="s">
+        <v>664</v>
+      </c>
+      <c r="H104" t="s">
+        <v>673</v>
+      </c>
+      <c r="I104" t="s">
+        <v>33</v>
+      </c>
+      <c r="J104">
+        <v>98236</v>
+      </c>
+      <c r="K104" t="s">
+        <v>190</v>
+      </c>
+      <c r="L104">
+        <v>47.992808799999999</v>
+      </c>
+      <c r="M104">
+        <v>-122.4006334</v>
+      </c>
+      <c r="N104" t="s">
+        <v>665</v>
+      </c>
+      <c r="O104" t="s">
+        <v>39</v>
+      </c>
+      <c r="R104" t="s">
+        <v>39</v>
+      </c>
+      <c r="S104" t="s">
+        <v>666</v>
+      </c>
+      <c r="U104" t="s">
+        <v>171</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>90105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>674</v>
+      </c>
+      <c r="C105">
+        <v>41</v>
+      </c>
+      <c r="D105" t="s">
+        <v>30</v>
+      </c>
+      <c r="F105" s="1">
+        <v>45395</v>
+      </c>
+      <c r="G105" t="s">
+        <v>667</v>
+      </c>
+      <c r="H105" t="s">
+        <v>46</v>
+      </c>
+      <c r="I105" t="s">
+        <v>33</v>
+      </c>
+      <c r="J105">
+        <v>98686</v>
+      </c>
+      <c r="K105" t="s">
+        <v>47</v>
+      </c>
+      <c r="L105">
+        <v>45.722899400000003</v>
+      </c>
+      <c r="M105">
+        <v>-122.6689896</v>
+      </c>
+      <c r="N105" t="s">
+        <v>615</v>
+      </c>
+      <c r="O105" t="s">
+        <v>36</v>
+      </c>
+      <c r="P105" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>207</v>
+      </c>
+      <c r="S105" t="s">
+        <v>668</v>
+      </c>
+      <c r="U105" t="s">
+        <v>52</v>
+      </c>
+      <c r="V105" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>90106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>669</v>
+      </c>
+      <c r="C106">
+        <v>38</v>
+      </c>
+      <c r="D106" t="s">
+        <v>30</v>
+      </c>
+      <c r="F106" s="1">
+        <v>45382</v>
+      </c>
+      <c r="G106" t="s">
+        <v>670</v>
+      </c>
+      <c r="H106" t="s">
+        <v>71</v>
+      </c>
+      <c r="I106" t="s">
+        <v>33</v>
+      </c>
+      <c r="J106">
+        <v>99201</v>
+      </c>
+      <c r="K106" t="s">
+        <v>71</v>
+      </c>
+      <c r="L106">
+        <v>47.666288199999997</v>
+      </c>
+      <c r="M106">
+        <v>-117.44106050000001</v>
+      </c>
+      <c r="N106" t="s">
+        <v>72</v>
+      </c>
+      <c r="O106" t="s">
+        <v>36</v>
+      </c>
+      <c r="P106" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>207</v>
+      </c>
+      <c r="S106" t="s">
+        <v>672</v>
+      </c>
+      <c r="U106" t="s">
+        <v>52</v>
+      </c>
+      <c r="V106" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>90107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>679</v>
+      </c>
+      <c r="C107">
+        <v>67</v>
+      </c>
+      <c r="D107" t="s">
+        <v>30</v>
+      </c>
+      <c r="E107" t="s">
+        <v>84</v>
+      </c>
+      <c r="F107" s="1">
+        <v>45399</v>
+      </c>
+      <c r="G107" t="s">
+        <v>677</v>
+      </c>
+      <c r="H107" t="s">
+        <v>682</v>
+      </c>
+      <c r="I107" t="s">
+        <v>33</v>
+      </c>
+      <c r="J107">
+        <v>98188</v>
+      </c>
+      <c r="K107" t="s">
+        <v>130</v>
+      </c>
+      <c r="L107">
+        <v>47.454423900000002</v>
+      </c>
+      <c r="M107">
+        <v>-122.263414</v>
+      </c>
+      <c r="N107" t="s">
+        <v>131</v>
+      </c>
+      <c r="O107" t="s">
+        <v>36</v>
+      </c>
+      <c r="P107" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>207</v>
+      </c>
+      <c r="S107" t="s">
+        <v>678</v>
+      </c>
+      <c r="U107" t="s">
+        <v>52</v>
+      </c>
+      <c r="V107" t="s">
+        <v>676</v>
+      </c>
+      <c r="AA107" t="s">
+        <v>680</v>
+      </c>
+      <c r="AB107" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>90108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>690</v>
+      </c>
+      <c r="C108">
+        <v>43</v>
+      </c>
+      <c r="D108" t="s">
+        <v>30</v>
+      </c>
+      <c r="E108" t="s">
+        <v>84</v>
+      </c>
+      <c r="F108" s="1">
+        <v>45380</v>
+      </c>
+      <c r="G108" t="s">
+        <v>685</v>
+      </c>
+      <c r="H108" t="s">
+        <v>727</v>
+      </c>
+      <c r="I108" t="s">
+        <v>33</v>
+      </c>
+      <c r="J108">
+        <v>99006</v>
+      </c>
+      <c r="K108" t="s">
+        <v>71</v>
+      </c>
+      <c r="L108">
+        <v>47.934369599999997</v>
+      </c>
+      <c r="M108">
+        <v>-117.5001469</v>
+      </c>
+      <c r="N108" t="s">
+        <v>684</v>
+      </c>
+      <c r="O108" t="s">
+        <v>36</v>
+      </c>
+      <c r="S108" t="s">
+        <v>686</v>
+      </c>
+      <c r="U108" t="s">
+        <v>52</v>
+      </c>
+      <c r="V108" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>688</v>
+      </c>
+      <c r="AB108" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>90109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>691</v>
+      </c>
+      <c r="C109">
+        <v>38</v>
+      </c>
+      <c r="D109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F109" s="1">
+        <v>45415</v>
+      </c>
+      <c r="G109" t="s">
+        <v>692</v>
+      </c>
+      <c r="H109" t="s">
+        <v>693</v>
+      </c>
+      <c r="I109" t="s">
+        <v>33</v>
+      </c>
+      <c r="J109">
+        <v>98362</v>
+      </c>
+      <c r="K109" t="s">
+        <v>306</v>
+      </c>
+      <c r="L109">
+        <v>48.120190000000001</v>
+      </c>
+      <c r="M109">
+        <v>-123.4376948</v>
+      </c>
+      <c r="N109" t="s">
+        <v>694</v>
+      </c>
+      <c r="O109" t="s">
+        <v>36</v>
+      </c>
+      <c r="P109" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>207</v>
+      </c>
+      <c r="S109" t="s">
+        <v>695</v>
+      </c>
+      <c r="U109" t="s">
+        <v>52</v>
+      </c>
+      <c r="V109" s="3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>90110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>697</v>
+      </c>
+      <c r="C110">
+        <v>31</v>
+      </c>
+      <c r="D110" t="s">
+        <v>30</v>
+      </c>
+      <c r="E110" t="s">
+        <v>44</v>
+      </c>
+      <c r="F110" s="1">
+        <v>45428</v>
+      </c>
+      <c r="G110" t="s">
+        <v>698</v>
+      </c>
+      <c r="H110" t="s">
+        <v>409</v>
+      </c>
+      <c r="I110" t="s">
+        <v>33</v>
+      </c>
+      <c r="J110">
+        <v>98201</v>
+      </c>
+      <c r="K110" t="s">
+        <v>190</v>
+      </c>
+      <c r="L110">
+        <v>47.970298100000001</v>
+      </c>
+      <c r="M110">
+        <v>-122.2198267</v>
+      </c>
+      <c r="N110" t="s">
+        <v>138</v>
+      </c>
+      <c r="O110" t="s">
+        <v>36</v>
+      </c>
+      <c r="P110" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>699</v>
+      </c>
+      <c r="S110" t="s">
+        <v>700</v>
+      </c>
+      <c r="U110" t="s">
+        <v>52</v>
+      </c>
+      <c r="V110" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>90111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>702</v>
+      </c>
+      <c r="C111">
+        <v>47</v>
+      </c>
+      <c r="D111" t="s">
+        <v>30</v>
+      </c>
+      <c r="F111" s="1">
+        <v>45435</v>
+      </c>
+      <c r="G111" t="s">
+        <v>706</v>
+      </c>
+      <c r="H111" t="s">
+        <v>145</v>
+      </c>
+      <c r="I111" t="s">
+        <v>33</v>
+      </c>
+      <c r="J111">
+        <v>99301</v>
+      </c>
+      <c r="K111" t="s">
+        <v>146</v>
+      </c>
+      <c r="L111">
+        <v>46.2428387</v>
+      </c>
+      <c r="M111">
+        <v>-119.1375922</v>
+      </c>
+      <c r="N111" t="s">
+        <v>147</v>
+      </c>
+      <c r="O111" t="s">
+        <v>36</v>
+      </c>
+      <c r="P111" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>703</v>
+      </c>
+      <c r="S111" t="s">
+        <v>707</v>
+      </c>
+      <c r="U111" t="s">
+        <v>52</v>
+      </c>
+      <c r="V111" t="s">
+        <v>704</v>
+      </c>
+      <c r="X111" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>705</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>90112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>708</v>
+      </c>
+      <c r="C112">
+        <v>48</v>
+      </c>
+      <c r="D112" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112" s="1">
+        <v>45436</v>
+      </c>
+      <c r="G112" t="s">
+        <v>710</v>
+      </c>
+      <c r="H112" t="s">
+        <v>711</v>
+      </c>
+      <c r="I112" t="s">
+        <v>33</v>
+      </c>
+      <c r="J112">
+        <v>98002</v>
+      </c>
+      <c r="K112" t="s">
+        <v>130</v>
+      </c>
+      <c r="L112">
+        <v>47.306731399999997</v>
+      </c>
+      <c r="M112">
+        <v>-122.2278898</v>
+      </c>
+      <c r="N112" t="s">
+        <v>712</v>
+      </c>
+      <c r="O112" t="s">
+        <v>36</v>
+      </c>
+      <c r="S112" t="s">
+        <v>713</v>
+      </c>
+      <c r="U112" t="s">
+        <v>52</v>
+      </c>
+      <c r="V112" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>90113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>725</v>
+      </c>
+      <c r="C113">
+        <v>43</v>
+      </c>
+      <c r="D113" t="s">
+        <v>30</v>
+      </c>
+      <c r="E113" t="s">
+        <v>84</v>
+      </c>
+      <c r="F113" s="1">
+        <v>45451</v>
+      </c>
+      <c r="G113" t="s">
+        <v>726</v>
+      </c>
+      <c r="H113" t="s">
+        <v>46</v>
+      </c>
+      <c r="I113" t="s">
+        <v>33</v>
+      </c>
+      <c r="J113">
+        <v>98661</v>
+      </c>
+      <c r="K113" t="s">
+        <v>47</v>
+      </c>
+      <c r="L113">
+        <v>45.621664600000003</v>
+      </c>
+      <c r="M113">
+        <v>-122.67751029999999</v>
+      </c>
+      <c r="N113" t="s">
+        <v>48</v>
+      </c>
+      <c r="O113" t="s">
+        <v>36</v>
+      </c>
+      <c r="P113" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>207</v>
+      </c>
+      <c r="S113" t="s">
+        <v>722</v>
+      </c>
+      <c r="U113" t="s">
+        <v>52</v>
+      </c>
+      <c r="V113" t="s">
+        <v>723</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>721</v>
+      </c>
+      <c r="AA113" t="s">
+        <v>724</v>
+      </c>
+      <c r="AB113" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>90114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>716</v>
+      </c>
+      <c r="C114">
+        <v>42</v>
+      </c>
+      <c r="D114" t="s">
+        <v>30</v>
+      </c>
+      <c r="F114" s="1">
+        <v>45460</v>
+      </c>
+      <c r="G114" t="s">
+        <v>717</v>
+      </c>
+      <c r="H114" t="s">
+        <v>46</v>
+      </c>
+      <c r="I114" t="s">
+        <v>33</v>
+      </c>
+      <c r="J114">
+        <v>98661</v>
+      </c>
+      <c r="K114" t="s">
+        <v>47</v>
+      </c>
+      <c r="L114">
+        <v>45.642665100000002</v>
+      </c>
+      <c r="M114">
+        <v>-122.6040588</v>
+      </c>
+      <c r="N114" t="s">
+        <v>48</v>
+      </c>
+      <c r="O114" t="s">
+        <v>36</v>
+      </c>
+      <c r="P114" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>207</v>
+      </c>
+      <c r="S114" t="s">
+        <v>719</v>
+      </c>
+      <c r="U114" t="s">
+        <v>52</v>
+      </c>
+      <c r="V114" t="s">
+        <v>718</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>720</v>
+      </c>
+      <c r="AA114" t="s">
+        <v>715</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>90115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>735</v>
+      </c>
+      <c r="D115" t="s">
+        <v>30</v>
+      </c>
+      <c r="E115" t="s">
+        <v>84</v>
+      </c>
+      <c r="F115" s="1">
+        <v>45475</v>
+      </c>
+      <c r="G115" t="s">
+        <v>728</v>
+      </c>
+      <c r="H115" t="s">
+        <v>153</v>
+      </c>
+      <c r="I115" t="s">
+        <v>33</v>
+      </c>
+      <c r="J115">
+        <v>98387</v>
+      </c>
+      <c r="K115" t="s">
+        <v>34</v>
+      </c>
+      <c r="L115">
+        <v>47.070533099999999</v>
+      </c>
+      <c r="M115">
+        <v>-122.4260957</v>
+      </c>
+      <c r="N115" t="s">
+        <v>35</v>
+      </c>
+      <c r="O115" t="s">
+        <v>36</v>
+      </c>
+      <c r="P115" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>207</v>
+      </c>
+      <c r="R115" t="s">
+        <v>39</v>
+      </c>
+      <c r="S115" t="s">
+        <v>729</v>
+      </c>
+      <c r="U115" t="s">
+        <v>52</v>
+      </c>
+      <c r="V115" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>90116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>736</v>
+      </c>
+      <c r="C116">
+        <v>42</v>
+      </c>
+      <c r="D116" t="s">
+        <v>30</v>
+      </c>
+      <c r="F116" s="1">
+        <v>45462</v>
+      </c>
+      <c r="G116" t="s">
+        <v>741</v>
+      </c>
+      <c r="H116" t="s">
+        <v>121</v>
+      </c>
+      <c r="I116" t="s">
+        <v>33</v>
+      </c>
+      <c r="J116">
+        <v>98422</v>
+      </c>
+      <c r="K116" t="s">
+        <v>34</v>
+      </c>
+      <c r="L116">
+        <v>47.2134541</v>
+      </c>
+      <c r="M116">
+        <v>-122.3876114</v>
+      </c>
+      <c r="N116" t="s">
+        <v>35</v>
+      </c>
+      <c r="O116" t="s">
+        <v>36</v>
+      </c>
+      <c r="R116" t="s">
+        <v>116</v>
+      </c>
+      <c r="S116" t="s">
+        <v>760</v>
+      </c>
+      <c r="U116" t="s">
+        <v>52</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="AD116" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>90117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>758</v>
+      </c>
+      <c r="C117">
+        <v>41</v>
+      </c>
+      <c r="D117" t="s">
+        <v>30</v>
+      </c>
+      <c r="F117" s="1">
+        <v>45486</v>
+      </c>
+      <c r="G117" t="s">
+        <v>757</v>
+      </c>
+      <c r="H117" t="s">
+        <v>137</v>
+      </c>
+      <c r="I117" t="s">
+        <v>33</v>
+      </c>
+      <c r="J117">
+        <v>98031</v>
+      </c>
+      <c r="K117" t="s">
+        <v>130</v>
+      </c>
+      <c r="L117">
+        <v>47.396026599999999</v>
+      </c>
+      <c r="M117">
+        <v>-122.2099808</v>
+      </c>
+      <c r="N117" t="s">
+        <v>227</v>
+      </c>
+      <c r="O117" t="s">
+        <v>39</v>
+      </c>
+      <c r="R117" t="s">
+        <v>39</v>
+      </c>
+      <c r="S117" t="s">
+        <v>732</v>
+      </c>
+      <c r="U117" t="s">
+        <v>171</v>
+      </c>
+      <c r="V117" s="3" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>90118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>748</v>
+      </c>
+      <c r="C118">
+        <v>67</v>
+      </c>
+      <c r="D118" t="s">
+        <v>168</v>
+      </c>
+      <c r="E118" t="s">
+        <v>84</v>
+      </c>
+      <c r="F118" s="1">
+        <v>45512</v>
+      </c>
+      <c r="G118" t="s">
+        <v>733</v>
+      </c>
+      <c r="H118" t="s">
+        <v>129</v>
+      </c>
+      <c r="I118" t="s">
+        <v>33</v>
+      </c>
+      <c r="J118">
+        <v>98108</v>
+      </c>
+      <c r="K118" t="s">
+        <v>130</v>
+      </c>
+      <c r="L118">
+        <v>47.563173999999997</v>
+      </c>
+      <c r="M118">
+        <v>-122.32303899999999</v>
+      </c>
+      <c r="N118" t="s">
+        <v>138</v>
+      </c>
+      <c r="O118" t="s">
+        <v>39</v>
+      </c>
+      <c r="R118" t="s">
+        <v>39</v>
+      </c>
+      <c r="S118" t="s">
+        <v>766</v>
+      </c>
+      <c r="U118" t="s">
+        <v>171</v>
+      </c>
+      <c r="V118" t="s">
+        <v>734</v>
+      </c>
+      <c r="Y118" t="s">
+        <v>749</v>
+      </c>
+      <c r="Z118" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>90119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>738</v>
+      </c>
+      <c r="C119">
+        <v>33</v>
+      </c>
+      <c r="D119" t="s">
+        <v>30</v>
+      </c>
+      <c r="E119" t="s">
+        <v>187</v>
+      </c>
+      <c r="F119" s="1">
+        <v>45532</v>
+      </c>
+      <c r="G119" t="s">
+        <v>739</v>
+      </c>
+      <c r="H119" t="s">
+        <v>137</v>
+      </c>
+      <c r="I119" t="s">
+        <v>33</v>
+      </c>
+      <c r="J119">
+        <v>98032</v>
+      </c>
+      <c r="K119" t="s">
+        <v>130</v>
+      </c>
+      <c r="L119">
+        <v>47.381646699999997</v>
+      </c>
+      <c r="M119">
+        <v>-122.2476602</v>
+      </c>
+      <c r="N119" t="s">
+        <v>227</v>
+      </c>
+      <c r="O119" t="s">
+        <v>36</v>
+      </c>
+      <c r="S119" t="s">
+        <v>761</v>
+      </c>
+      <c r="U119" t="s">
+        <v>763</v>
+      </c>
+      <c r="V119" t="s">
+        <v>762</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="120" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>90120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>786</v>
+      </c>
+      <c r="C120" s="5">
+        <v>48</v>
+      </c>
+      <c r="D120" t="s">
+        <v>30</v>
+      </c>
+      <c r="E120" t="s">
+        <v>84</v>
+      </c>
+      <c r="F120" s="1">
+        <v>45497</v>
+      </c>
+      <c r="G120" t="s">
+        <v>740</v>
+      </c>
+      <c r="H120" t="s">
+        <v>32</v>
+      </c>
+      <c r="I120" t="s">
+        <v>33</v>
+      </c>
+      <c r="J120">
+        <v>98321</v>
+      </c>
+      <c r="K120" t="s">
+        <v>34</v>
+      </c>
+      <c r="L120">
+        <v>47.1508477</v>
+      </c>
+      <c r="M120">
+        <v>-122.10860599999999</v>
+      </c>
+      <c r="N120" t="s">
+        <v>35</v>
+      </c>
+      <c r="O120" t="s">
+        <v>36</v>
+      </c>
+      <c r="P120" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>207</v>
+      </c>
+      <c r="S120" t="s">
+        <v>752</v>
+      </c>
+      <c r="U120" t="s">
+        <v>52</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>90121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>787</v>
+      </c>
+      <c r="C121">
+        <v>57</v>
+      </c>
+      <c r="D121" t="s">
+        <v>30</v>
+      </c>
+      <c r="E121" t="s">
+        <v>84</v>
+      </c>
+      <c r="F121" s="1">
+        <v>45492</v>
+      </c>
+      <c r="G121" t="s">
+        <v>747</v>
+      </c>
+      <c r="H121" t="s">
+        <v>742</v>
+      </c>
+      <c r="I121" t="s">
+        <v>33</v>
+      </c>
+      <c r="J121">
+        <v>99114</v>
+      </c>
+      <c r="K121" t="s">
+        <v>744</v>
+      </c>
+      <c r="L121">
+        <v>48.580203400000002</v>
+      </c>
+      <c r="M121">
+        <v>-117.9693434</v>
+      </c>
+      <c r="N121" t="s">
+        <v>746</v>
+      </c>
+      <c r="O121" t="s">
+        <v>36</v>
+      </c>
+      <c r="P121" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>49</v>
+      </c>
+      <c r="S121" t="s">
+        <v>751</v>
+      </c>
+      <c r="U121" t="s">
+        <v>52</v>
+      </c>
+      <c r="V121" s="3" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>90122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>737</v>
+      </c>
+      <c r="C122">
+        <v>38</v>
+      </c>
+      <c r="D122" t="s">
+        <v>30</v>
+      </c>
+      <c r="F122" s="1">
+        <v>45488</v>
+      </c>
+      <c r="G122" t="s">
+        <v>745</v>
+      </c>
+      <c r="H122" t="s">
+        <v>743</v>
+      </c>
+      <c r="I122" t="s">
+        <v>33</v>
+      </c>
+      <c r="J122">
+        <v>98338</v>
+      </c>
+      <c r="K122" t="s">
+        <v>34</v>
+      </c>
+      <c r="L122">
+        <v>47.020754199999999</v>
+      </c>
+      <c r="M122">
+        <v>-122.3413482</v>
+      </c>
+      <c r="N122" t="s">
+        <v>35</v>
+      </c>
+      <c r="O122" t="s">
+        <v>36</v>
+      </c>
+      <c r="R122" t="s">
+        <v>39</v>
+      </c>
+      <c r="S122" t="s">
+        <v>756</v>
+      </c>
+      <c r="U122" t="s">
+        <v>89</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>90123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>767</v>
+      </c>
+      <c r="C123">
+        <v>70</v>
+      </c>
+      <c r="D123" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" t="s">
+        <v>84</v>
+      </c>
+      <c r="F123" s="1">
+        <v>45542</v>
+      </c>
+      <c r="G123" t="s">
+        <v>770</v>
+      </c>
+      <c r="H123" t="s">
+        <v>269</v>
+      </c>
+      <c r="I123" t="s">
+        <v>33</v>
+      </c>
+      <c r="J123">
+        <v>98501</v>
+      </c>
+      <c r="K123" t="s">
+        <v>64</v>
+      </c>
+      <c r="L123">
+        <v>47.041699199999996</v>
+      </c>
+      <c r="M123">
+        <v>-122.84954310000001</v>
+      </c>
+      <c r="N123" t="s">
+        <v>181</v>
+      </c>
+      <c r="O123" t="s">
+        <v>39</v>
+      </c>
+      <c r="R123" t="s">
+        <v>39</v>
+      </c>
+      <c r="S123" t="s">
+        <v>769</v>
+      </c>
+      <c r="U123" t="s">
+        <v>171</v>
+      </c>
+      <c r="V123" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>90124</v>
+      </c>
+      <c r="C124">
+        <v>19</v>
+      </c>
+      <c r="D124" t="s">
+        <v>30</v>
+      </c>
+      <c r="F124" s="1">
+        <v>45549</v>
+      </c>
+      <c r="G124" t="s">
+        <v>773</v>
+      </c>
+      <c r="H124" t="s">
+        <v>190</v>
+      </c>
+      <c r="I124" t="s">
+        <v>33</v>
+      </c>
+      <c r="J124">
+        <v>98258</v>
+      </c>
+      <c r="K124" t="s">
+        <v>190</v>
+      </c>
+      <c r="L124">
+        <v>48.060391199999998</v>
+      </c>
+      <c r="M124">
+        <v>-122.11364639999999</v>
+      </c>
+      <c r="N124" t="s">
+        <v>771</v>
+      </c>
+      <c r="O124" t="s">
+        <v>39</v>
+      </c>
+      <c r="R124" t="s">
+        <v>39</v>
+      </c>
+      <c r="S124" t="s">
+        <v>774</v>
+      </c>
+      <c r="U124" t="s">
+        <v>171</v>
+      </c>
+      <c r="V124" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>90125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>799</v>
+      </c>
+      <c r="C125">
+        <v>35</v>
+      </c>
+      <c r="D125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E125" t="s">
+        <v>800</v>
+      </c>
+      <c r="F125" s="1">
+        <v>45549</v>
+      </c>
+      <c r="G125" t="s">
+        <v>779</v>
+      </c>
+      <c r="H125" t="s">
+        <v>775</v>
+      </c>
+      <c r="I125" t="s">
+        <v>33</v>
+      </c>
+      <c r="J125">
+        <v>98390</v>
+      </c>
+      <c r="K125" t="s">
+        <v>34</v>
+      </c>
+      <c r="L125">
+        <v>47.200977399999999</v>
+      </c>
+      <c r="M125">
+        <v>-122.24831690000001</v>
+      </c>
+      <c r="N125" t="s">
+        <v>776</v>
+      </c>
+      <c r="O125" t="s">
+        <v>36</v>
+      </c>
+      <c r="P125" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>49</v>
+      </c>
+      <c r="S125" t="s">
+        <v>777</v>
+      </c>
+      <c r="U125" t="s">
+        <v>52</v>
+      </c>
+      <c r="V125" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="AE125" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>90126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>780</v>
+      </c>
+      <c r="C126">
+        <v>45</v>
+      </c>
+      <c r="D126" t="s">
+        <v>30</v>
+      </c>
+      <c r="E126" t="s">
+        <v>84</v>
+      </c>
+      <c r="F126" s="1">
+        <v>45272</v>
+      </c>
+      <c r="G126" t="s">
+        <v>782</v>
+      </c>
+      <c r="H126" t="s">
+        <v>121</v>
+      </c>
+      <c r="I126" t="s">
+        <v>33</v>
+      </c>
+      <c r="J126">
+        <v>98443</v>
+      </c>
+      <c r="K126" t="s">
+        <v>34</v>
+      </c>
+      <c r="L126">
+        <v>47.217165799999997</v>
+      </c>
+      <c r="M126">
+        <v>-122.3795559</v>
+      </c>
+      <c r="N126" t="s">
+        <v>35</v>
+      </c>
+      <c r="O126" t="s">
+        <v>36</v>
+      </c>
+      <c r="P126" t="s">
+        <v>37</v>
+      </c>
+      <c r="R126" t="s">
+        <v>39</v>
+      </c>
+      <c r="S126" t="s">
+        <v>783</v>
+      </c>
+      <c r="U126" t="s">
+        <v>89</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>781</v>
+      </c>
+      <c r="AD126" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>90127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>790</v>
+      </c>
+      <c r="C127">
+        <v>72</v>
+      </c>
+      <c r="D127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E127" t="s">
+        <v>84</v>
+      </c>
+      <c r="F127" s="1">
+        <v>45388</v>
+      </c>
+      <c r="G127" t="s">
+        <v>792</v>
+      </c>
+      <c r="H127" t="s">
+        <v>793</v>
+      </c>
+      <c r="I127" t="s">
+        <v>33</v>
+      </c>
+      <c r="J127">
+        <v>98584</v>
+      </c>
+      <c r="K127" t="s">
+        <v>794</v>
+      </c>
+      <c r="L127">
+        <v>47.142985500000002</v>
+      </c>
+      <c r="M127">
+        <v>-123.0974449</v>
+      </c>
+      <c r="N127" t="s">
+        <v>138</v>
+      </c>
+      <c r="O127" t="s">
+        <v>39</v>
+      </c>
+      <c r="S127" t="s">
+        <v>795</v>
+      </c>
+      <c r="U127" t="s">
+        <v>797</v>
+      </c>
+      <c r="V127" s="3" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>90128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>791</v>
+      </c>
+      <c r="C128">
+        <v>49</v>
+      </c>
+      <c r="D128" t="s">
+        <v>168</v>
+      </c>
+      <c r="E128" t="s">
+        <v>84</v>
+      </c>
+      <c r="F128" s="1">
+        <v>45388</v>
+      </c>
+      <c r="G128" t="s">
+        <v>792</v>
+      </c>
+      <c r="H128" t="s">
+        <v>793</v>
+      </c>
+      <c r="I128" t="s">
+        <v>33</v>
+      </c>
+      <c r="J128">
+        <v>98584</v>
+      </c>
+      <c r="K128" t="s">
+        <v>794</v>
+      </c>
+      <c r="L128">
+        <v>47.142985500000002</v>
+      </c>
+      <c r="M128">
+        <v>-123.0974449</v>
+      </c>
+      <c r="N128" t="s">
+        <v>138</v>
+      </c>
+      <c r="O128" t="s">
+        <v>39</v>
+      </c>
+      <c r="S128" t="s">
+        <v>796</v>
+      </c>
+      <c r="U128" t="s">
+        <v>797</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="129" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>90129</v>
+      </c>
+      <c r="B129" t="s">
+        <v>819</v>
+      </c>
+      <c r="C129">
+        <v>18</v>
+      </c>
+      <c r="D129" t="s">
+        <v>30</v>
+      </c>
+      <c r="E129" t="s">
+        <v>44</v>
+      </c>
+      <c r="F129" s="1">
+        <v>45557</v>
+      </c>
+      <c r="G129" t="s">
+        <v>801</v>
+      </c>
+      <c r="H129" t="s">
+        <v>409</v>
+      </c>
+      <c r="I129" t="s">
+        <v>33</v>
+      </c>
+      <c r="J129">
+        <v>98203</v>
+      </c>
+      <c r="K129" t="s">
+        <v>190</v>
+      </c>
+      <c r="L129">
+        <v>47.929929199999997</v>
+      </c>
+      <c r="M129">
+        <v>-122.23107</v>
+      </c>
+      <c r="N129" t="s">
+        <v>420</v>
+      </c>
+      <c r="O129" t="s">
+        <v>39</v>
+      </c>
+      <c r="P129" t="s">
+        <v>37</v>
+      </c>
+      <c r="R129" t="s">
+        <v>39</v>
+      </c>
+      <c r="S129" t="s">
+        <v>802</v>
+      </c>
+      <c r="U129" t="s">
+        <v>41</v>
+      </c>
+      <c r="V129" t="s">
+        <v>820</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>814</v>
+      </c>
+      <c r="AE129" s="4" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>90130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>803</v>
+      </c>
+      <c r="C130">
+        <v>36</v>
+      </c>
+      <c r="D130" t="s">
+        <v>30</v>
+      </c>
+      <c r="F130" s="1">
+        <v>45555</v>
+      </c>
+      <c r="G130" t="s">
+        <v>805</v>
+      </c>
+      <c r="H130" t="s">
+        <v>269</v>
+      </c>
+      <c r="I130" t="s">
+        <v>33</v>
+      </c>
+      <c r="J130">
+        <v>98501</v>
+      </c>
+      <c r="K130" t="s">
+        <v>64</v>
+      </c>
+      <c r="L130">
+        <v>47.014322</v>
+      </c>
+      <c r="M130">
+        <v>-122.844269</v>
+      </c>
+      <c r="N130" t="s">
+        <v>804</v>
+      </c>
+      <c r="O130" t="s">
+        <v>39</v>
+      </c>
+      <c r="R130" t="s">
+        <v>139</v>
+      </c>
+      <c r="S130" t="s">
+        <v>806</v>
+      </c>
+      <c r="U130" t="s">
+        <v>171</v>
+      </c>
+      <c r="V130" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>90131</v>
+      </c>
+      <c r="B131" t="s">
+        <v>822</v>
+      </c>
+      <c r="C131">
+        <v>56</v>
+      </c>
+      <c r="D131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F131" s="1">
+        <v>45562</v>
+      </c>
+      <c r="G131" t="s">
+        <v>823</v>
+      </c>
+      <c r="H131" t="s">
+        <v>46</v>
+      </c>
+      <c r="I131" t="s">
+        <v>33</v>
+      </c>
+      <c r="J131">
+        <v>98661</v>
+      </c>
+      <c r="K131" t="s">
+        <v>47</v>
+      </c>
+      <c r="L131">
+        <v>45.6739125</v>
+      </c>
+      <c r="M131">
+        <v>-122.61947189999999</v>
+      </c>
+      <c r="N131" t="s">
+        <v>809</v>
+      </c>
+      <c r="O131" t="s">
+        <v>36</v>
+      </c>
+      <c r="P131" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>207</v>
+      </c>
+      <c r="S131" t="s">
+        <v>810</v>
+      </c>
+      <c r="U131" t="s">
+        <v>52</v>
+      </c>
+      <c r="V131" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>90132</v>
+      </c>
+      <c r="D132" t="s">
+        <v>30</v>
+      </c>
+      <c r="F132" s="1">
+        <v>45564</v>
+      </c>
+      <c r="G132" t="s">
+        <v>813</v>
+      </c>
+      <c r="H132" t="s">
+        <v>409</v>
+      </c>
+      <c r="I132" t="s">
+        <v>33</v>
+      </c>
+      <c r="J132">
+        <v>98201</v>
+      </c>
+      <c r="K132" t="s">
+        <v>190</v>
+      </c>
+      <c r="L132">
+        <v>47.992366400000002</v>
+      </c>
+      <c r="M132">
+        <v>-122.200962</v>
+      </c>
+      <c r="N132" t="s">
+        <v>138</v>
+      </c>
+      <c r="O132" t="s">
+        <v>39</v>
+      </c>
+      <c r="R132" t="s">
+        <v>39</v>
+      </c>
+      <c r="S132" t="s">
+        <v>818</v>
+      </c>
+      <c r="U132" t="s">
+        <v>171</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="Y132" t="s">
+        <v>812</v>
+      </c>
+      <c r="Z132" t="s">
+        <v>817</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9586,10 +11857,20 @@
     <hyperlink ref="V100" r:id="rId2" xr:uid="{F3A7DA00-F8A5-47D8-9653-80C07B327419}"/>
     <hyperlink ref="V102" r:id="rId3" xr:uid="{D410200E-9C82-42EC-8872-FC44A64A0761}"/>
     <hyperlink ref="V103" r:id="rId4" xr:uid="{8E96F9EF-81DE-465A-9CAE-084D6FCF0C68}"/>
+    <hyperlink ref="V104" r:id="rId5" xr:uid="{E56DD1EB-FD4A-459E-8CE4-13E80335B609}"/>
+    <hyperlink ref="V108" r:id="rId6" xr:uid="{D528F3D6-B85E-4E25-9F17-2FC22AA53BE0}"/>
+    <hyperlink ref="V109" r:id="rId7" xr:uid="{82315842-37E2-4E90-A39A-CF1CA94C10A9}"/>
+    <hyperlink ref="V115" r:id="rId8" xr:uid="{D4A88BDF-65AA-41E5-A416-922436E6084C}"/>
+    <hyperlink ref="V125" r:id="rId9" xr:uid="{A3F5670F-1A81-4C57-A5D1-6E88AC528848}"/>
+    <hyperlink ref="V126" r:id="rId10" xr:uid="{56DF61C4-ADE9-4481-A0E0-16C6BA0253B6}"/>
+    <hyperlink ref="V127" r:id="rId11" xr:uid="{2F5E5ECD-7633-4256-B7BA-C30080DEE1F7}"/>
+    <hyperlink ref="V128" r:id="rId12" xr:uid="{6816D393-9C44-40AF-B65E-D44C362F32C4}"/>
+    <hyperlink ref="V132" r:id="rId13" xr:uid="{7FCFF8A8-6CD4-4850-B07C-123343A80752}"/>
+    <hyperlink ref="AE129" r:id="rId14" xr:uid="{2D3C2A56-A3DE-4A76-8C05-17EBDCDE9850}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final updates to FE-WaPo Repo.  Future work will rely on MPV in a separate respository.
</commit_message>
<xml_diff>
--- a/Data/Raw/fe_newnames.xlsx
+++ b/Data/Raw/fe_newnames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\fewapo\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928D2619-80F8-4953-AB4F-B0A957E51A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F60B79-32D8-4600-851F-66D134481B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3783,8 +3783,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AE158" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:AE158" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE157">
-    <sortCondition ref="F1:F157"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE158">
+    <sortCondition ref="F1:F158"/>
   </sortState>
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Unique ID" dataDxfId="30"/>
@@ -4123,10 +4123,10 @@
   <dimension ref="A1:AE158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R116" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U132" sqref="U132"/>
+      <selection pane="bottomRight" activeCell="F146" sqref="F146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -14257,59 +14257,59 @@
         <v>944</v>
       </c>
     </row>
-    <row r="156" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A156">
+    <row r="156" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="6">
         <v>90150</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F156" s="1">
+      <c r="F156" s="7">
         <v>45740</v>
       </c>
-      <c r="G156" t="s">
+      <c r="G156" s="6" t="s">
         <v>902</v>
       </c>
-      <c r="H156" t="s">
+      <c r="H156" s="6" t="s">
         <v>901</v>
       </c>
-      <c r="I156" t="s">
-        <v>33</v>
-      </c>
-      <c r="J156">
+      <c r="I156" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J156" s="6">
         <v>99157</v>
       </c>
-      <c r="K156" t="s">
+      <c r="K156" s="6" t="s">
         <v>737</v>
       </c>
-      <c r="L156">
+      <c r="L156" s="6">
         <v>48.828353</v>
       </c>
-      <c r="M156">
+      <c r="M156" s="6">
         <v>-117.9129664</v>
       </c>
-      <c r="N156" t="s">
+      <c r="N156" s="6" t="s">
         <v>739</v>
       </c>
-      <c r="O156" t="s">
+      <c r="O156" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="P156" t="s">
+      <c r="P156" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q156" t="s">
+      <c r="Q156" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="S156" t="s">
+      <c r="S156" s="6" t="s">
         <v>903</v>
       </c>
-      <c r="U156" t="s">
+      <c r="U156" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V156" t="s">
+      <c r="V156" s="6" t="s">
         <v>904</v>
       </c>
-      <c r="AD156" t="s">
+      <c r="AD156" s="6" t="s">
         <v>905</v>
       </c>
     </row>

</xml_diff>